<commit_message>
implementation of the organization
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9750" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9985" uniqueCount="382">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1169,6 +1169,12 @@
   <si>
     <t>328A</t>
   </si>
+  <si>
+    <t>8/01/16</t>
+  </si>
+  <si>
+    <t>8/1/16</t>
+  </si>
 </sst>
 </file>
 
@@ -2011,7 +2017,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H1767"/>
+  <dimension ref="A1:H1811"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1306" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1335" sqref="A1335:XFD1335"/>
@@ -38286,7 +38292,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="1761" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1761" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1761" s="70" t="s">
         <v>27</v>
       </c>
@@ -38306,7 +38312,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1762" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1762" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1762" s="70" t="s">
         <v>27</v>
       </c>
@@ -38326,7 +38332,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1763" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1763" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1763" s="48" t="s">
         <v>27</v>
       </c>
@@ -38343,7 +38349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1764" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1764" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1764" s="70" t="s">
         <v>27</v>
       </c>
@@ -38363,7 +38369,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1765" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1765" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1765" s="48" t="s">
         <v>27</v>
       </c>
@@ -38380,7 +38386,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1766" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1766" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1766" s="48" t="s">
         <v>27</v>
       </c>
@@ -38397,7 +38403,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="1767" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1767" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1767" s="48" t="s">
         <v>27</v>
       </c>
@@ -38411,6 +38417,804 @@
         <v>25</v>
       </c>
       <c r="F1767" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1768" spans="2:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1768" s="91"/>
+      <c r="D1768" s="92"/>
+      <c r="F1768" s="93"/>
+      <c r="G1768" s="94"/>
+      <c r="H1768" s="95"/>
+    </row>
+    <row r="1769" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1769" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1769" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1769" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1769" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1769" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1770" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1770" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1770" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1770" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1770" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1770" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1771" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1771" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1771" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1771" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1771" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1771" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1772" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1772" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1772" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1772" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1772" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1772" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1772" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1773" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1773" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1773" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1773" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1773" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1773" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1773" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1774" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1774" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1774" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1774" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1774" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1774" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="1775" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1775" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1775" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1775" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1775" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1775" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1775" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1776" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1776" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1776" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1776" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1776" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1776" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1776" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1777" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1777" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1777" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1777" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1777" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1777" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1778" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1778" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1778" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1778" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1778" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1778" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="1779" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1779" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1779" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1779" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1779" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1779" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="1780" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1780" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1780" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1780" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1780" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1780" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1781" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1781" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1781" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1781" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1781" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1781" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1782" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1782" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1782" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1782" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1782" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1782" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1783" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1783" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1783" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1783" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1783" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1783" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1783" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1784" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1784" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1784" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1784" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1784" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1784" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1785" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1785" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1785" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1785" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1785" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1785" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1786" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1786" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1786" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1786" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1786" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1786" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1786" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1787" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1787" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1787" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1787" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1787" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1787" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1787" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1788" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1788" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1788" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1788" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1788" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1788" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1789" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1789" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1789" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1789" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1789" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1789" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1790" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1790" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1790" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1790" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1790" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1790" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1790" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1791" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1791" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1791" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1791" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1791" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1791" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="1792" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1792" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1792" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1792" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1792" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1792" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="1793" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1793" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1793" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1793" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1793" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1793" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1793" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1794" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1794" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1794" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1794" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1794" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1794" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1794" s="97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1795" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1795" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1795" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1795" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1795" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1795" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1796" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1796" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1796" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1796" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1796" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1796" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1797" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1797" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1797" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1797" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1797" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1797" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1797" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1798" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1798" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1798" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1798" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1798" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1798" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1798" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1799" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1799" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1799" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1799" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1799" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1799" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1799" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1800" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1800" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1800" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1800" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1800" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1800" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1800" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1801" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1801" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1801" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1801" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1801" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1801" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1801" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1802" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1802" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1802" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1802" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1802" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1802" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1802" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1803" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1803" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1803" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1803" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1803" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1803" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1803" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1804" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1804" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1804" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1804" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1804" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1804" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1805" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1805" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1805" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1805" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1805" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1805" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1805" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1806" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1806" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1806" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1806" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1806" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1806" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1806" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1807" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1807" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1807" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1807" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1807" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1807" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1808" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1808" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1808" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1808" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1808" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1808" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1808" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1809" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1809" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1809" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1809" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1809" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1809" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1810" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1810" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1810" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1810" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1810" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1810" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="1811" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1811" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1811" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1811" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1811" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1811" s="13" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a format bug
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9750" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9985" uniqueCount="381">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1169,6 +1169,9 @@
   <si>
     <t>328A</t>
   </si>
+  <si>
+    <t>8/01/16</t>
+  </si>
 </sst>
 </file>
 
@@ -2011,7 +2014,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H1767"/>
+  <dimension ref="A1:H1811"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1306" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1335" sqref="A1335:XFD1335"/>
@@ -38286,7 +38289,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="1761" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1761" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1761" s="70" t="s">
         <v>27</v>
       </c>
@@ -38306,7 +38309,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1762" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1762" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1762" s="70" t="s">
         <v>27</v>
       </c>
@@ -38326,7 +38329,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1763" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1763" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1763" s="48" t="s">
         <v>27</v>
       </c>
@@ -38343,7 +38346,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1764" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1764" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1764" s="70" t="s">
         <v>27</v>
       </c>
@@ -38363,7 +38366,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1765" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1765" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1765" s="48" t="s">
         <v>27</v>
       </c>
@@ -38380,7 +38383,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1766" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1766" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1766" s="48" t="s">
         <v>27</v>
       </c>
@@ -38397,7 +38400,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="1767" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1767" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1767" s="48" t="s">
         <v>27</v>
       </c>
@@ -38411,6 +38414,804 @@
         <v>25</v>
       </c>
       <c r="F1767" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1768" spans="2:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1768" s="91"/>
+      <c r="D1768" s="92"/>
+      <c r="F1768" s="93"/>
+      <c r="G1768" s="94"/>
+      <c r="H1768" s="95"/>
+    </row>
+    <row r="1769" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1769" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1769" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1769" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1769" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1769" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1770" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1770" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1770" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1770" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1770" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1770" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1771" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1771" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1771" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1771" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1771" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1771" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1772" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1772" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1772" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1772" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1772" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1772" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1772" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1773" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1773" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1773" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1773" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1773" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1773" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1773" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1774" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1774" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1774" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1774" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1774" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1774" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="1775" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1775" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1775" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1775" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1775" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1775" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1775" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1776" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1776" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1776" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1776" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1776" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1776" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1776" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1777" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1777" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1777" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1777" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1777" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1777" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1778" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1778" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1778" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1778" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1778" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1778" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="1779" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1779" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1779" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1779" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1779" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1779" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="1780" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1780" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1780" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1780" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1780" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1780" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1781" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1781" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1781" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1781" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1781" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1781" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1782" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1782" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1782" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1782" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1782" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1782" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1783" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1783" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1783" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1783" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1783" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1783" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1783" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1784" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1784" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1784" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1784" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1784" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1784" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1785" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1785" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1785" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1785" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1785" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1785" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1786" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1786" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1786" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1786" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1786" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1786" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1786" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1787" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1787" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1787" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1787" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1787" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1787" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1787" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1788" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1788" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1788" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1788" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1788" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1788" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1789" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1789" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1789" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1789" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1789" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1789" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1790" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1790" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1790" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1790" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1790" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1790" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1790" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1791" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1791" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1791" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1791" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1791" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1791" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="1792" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1792" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1792" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1792" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1792" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1792" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="1793" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1793" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1793" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1793" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1793" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1793" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1793" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1794" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1794" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1794" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1794" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1794" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1794" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1794" s="97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1795" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1795" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1795" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1795" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1795" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1795" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1796" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1796" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1796" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1796" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1796" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1796" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1797" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1797" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1797" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1797" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1797" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1797" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1797" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1798" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1798" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1798" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1798" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1798" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1798" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1798" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1799" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1799" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1799" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1799" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1799" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1799" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1799" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1800" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1800" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1800" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1800" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1800" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1800" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1800" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1801" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1801" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1801" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1801" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1801" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1801" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1801" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1802" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1802" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1802" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1802" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1802" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1802" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1802" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1803" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1803" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1803" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1803" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1803" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1803" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1803" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1804" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1804" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1804" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1804" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1804" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1804" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1805" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1805" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1805" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1805" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1805" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1805" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1805" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1806" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1806" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1806" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1806" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1806" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1806" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1806" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1807" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1807" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1807" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1807" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1807" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1807" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1808" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1808" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1808" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1808" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1808" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1808" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1808" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1809" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1809" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1809" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1809" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1809" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1809" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1810" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1810" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1810" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1810" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1810" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1810" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="1811" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1811" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1811" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1811" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1811" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1811" s="13" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ranking done for 2,3, and 4 zones.
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13907" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14445" uniqueCount="382">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2017,7 +2017,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H2553"/>
+  <dimension ref="A1:H2653"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1306" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1335" sqref="A1335:XFD1335"/>
@@ -52398,7 +52398,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2545" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2545" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2545" s="48" t="s">
         <v>27</v>
       </c>
@@ -52415,7 +52415,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2546" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2546" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2546" s="70" t="s">
         <v>27</v>
       </c>
@@ -52435,7 +52435,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2547" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2547" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2547" s="70" t="s">
         <v>27</v>
       </c>
@@ -52455,7 +52455,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2548" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2548" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2548" s="48" t="s">
         <v>27</v>
       </c>
@@ -52472,7 +52472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2549" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2549" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2549" s="70" t="s">
         <v>27</v>
       </c>
@@ -52492,7 +52492,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2550" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2550" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2550" s="48" t="s">
         <v>27</v>
       </c>
@@ -52509,7 +52509,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2551" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2551" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2551" s="48" t="s">
         <v>27</v>
       </c>
@@ -52526,7 +52526,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="2552" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2552" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2552" s="48" t="s">
         <v>27</v>
       </c>
@@ -52543,7 +52543,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2553" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2553" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2553" s="70" t="s">
         <v>27</v>
       </c>
@@ -52560,6 +52560,1830 @@
         <v>297</v>
       </c>
       <c r="G2553" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2554" spans="2:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2554" s="91"/>
+      <c r="D2554" s="92"/>
+      <c r="F2554" s="93"/>
+      <c r="G2554" s="94"/>
+      <c r="H2554" s="95"/>
+    </row>
+    <row r="2555" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2555" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2555" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2555" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2555" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2555" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2556" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2556" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2556" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2556" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2556" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2556" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2557" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2557" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2557" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2557" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2557" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2557" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2558" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2558" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2558" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2558" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2558" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2558" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2558" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2559" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2559" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2559" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2559" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2559" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2559" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2559" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2560" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2560" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2560" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2560" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2560" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2560" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2561" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2561" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2561" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2561" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2561" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2561" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2561" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2562" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2562" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2562" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2562" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2562" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2562" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2562" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2563" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2563" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2563" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2563" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2563" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2563" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2564" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2564" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2564" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2564" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2564" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2564" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2565" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2565" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2565" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2565" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2565" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2565" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2566" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2566" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2566" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2566" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2566" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2566" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2567" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2567" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2567" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2567" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2567" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2567" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2568" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2568" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2568" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2568" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2568" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2568" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2569" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2569" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2569" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2569" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2569" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2569" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2569" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2570" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2570" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2570" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2570" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2570" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2570" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2571" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2571" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2571" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2571" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2571" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2571" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2572" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2572" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2572" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2572" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2572" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2572" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2572" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2573" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2573" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2573" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2573" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2573" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2573" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2574" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2574" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2574" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2574" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2574" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2574" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2575" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2575" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2575" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2575" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2575" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2575" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2576" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2576" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2576" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2576" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2576" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2576" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2576" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2577" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2577" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2577" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2577" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2577" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2577" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2578" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2578" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2578" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2578" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2578" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2578" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2579" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2579" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2579" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2579" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2579" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2579" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2579" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2580" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2580" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2580" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2580" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2580" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2580" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2580" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2581" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2581" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2581" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2581" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2581" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2581" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2581" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2582" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2582" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2582" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2582" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2582" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2582" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2582" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2583" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2583" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2583" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2583" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2583" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2583" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2583" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2584" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2584" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2584" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2584" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2584" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2584" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2584" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2585" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2585" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2585" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2585" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2585" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2585" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2585" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2586" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2586" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2586" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2586" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2586" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2586" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2586" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2587" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2587" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2587" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2587" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2587" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2587" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2588" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2588" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2588" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2588" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2588" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2588" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2588" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2589" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2589" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2589" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2589" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2589" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2589" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2589" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2590" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2590" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2590" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2590" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2590" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2590" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2591" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2591" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2591" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2591" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2591" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2591" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2592" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2592" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2592" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2592" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2592" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2592" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2592" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2593" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2593" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2593" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2593" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2593" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2593" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2594" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2594" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2594" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2594" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2594" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2594" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2594" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2595" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2595" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2595" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2595" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2595" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2595" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2595" s="97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2596" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2596" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2596" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2596" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2596" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2596" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2597" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2597" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2597" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2597" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2597" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2597" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2597" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2598" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2598" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2598" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2598" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2598" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2598" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G2598" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2599" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2599" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2599" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2599" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2599" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2599" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2600" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2600" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2600" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2600" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2600" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2600" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2601" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2601" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2601" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2601" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2601" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2601" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2602" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2602" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2602" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2602" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2602" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2602" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2602" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2603" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2603" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2603" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2603" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2603" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2603" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2603" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2604" spans="2:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2604" s="91"/>
+      <c r="D2604" s="92"/>
+      <c r="F2604" s="93"/>
+      <c r="G2604" s="94"/>
+      <c r="H2604" s="95"/>
+    </row>
+    <row r="2605" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2605" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2605" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2605" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2605" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2605" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2606" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2606" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2606" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2606" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2606" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2606" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2607" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2607" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2607" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2607" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2607" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2607" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2608" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2608" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2608" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2608" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2608" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2608" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2608" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2609" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2609" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2609" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2609" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2609" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2609" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2609" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2610" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2610" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2610" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2610" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2610" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2610" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2611" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2611" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2611" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2611" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2611" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2611" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2611" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2612" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2612" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2612" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2612" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2612" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2612" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2612" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2613" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2613" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2613" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2613" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2613" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2613" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2614" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2614" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2614" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2614" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2614" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2614" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2615" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2615" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2615" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2615" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2615" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2615" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2616" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2616" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2616" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2616" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2616" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2616" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2617" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2617" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2617" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2617" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2617" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2617" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2618" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2618" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2618" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2618" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2618" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2618" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2619" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2619" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2619" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2619" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2619" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2619" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2619" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2620" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2620" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2620" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2620" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2620" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2620" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2621" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2621" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2621" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2621" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2621" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2621" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2622" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2622" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2622" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2622" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2622" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2622" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2622" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2623" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2623" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2623" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2623" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2623" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2623" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2624" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2624" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2624" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2624" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2624" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2624" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2625" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2625" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2625" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2625" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2625" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2625" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2625" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2626" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2626" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2626" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2626" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2626" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2626" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2627" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2627" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2627" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2627" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2627" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2627" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2628" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2628" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2628" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2628" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2628" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2628" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2628" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2629" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2629" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2629" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2629" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2629" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2629" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2630" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2630" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2630" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2630" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2630" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2630" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2630" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2631" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2631" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2631" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2631" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2631" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2631" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2631" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2632" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2632" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2632" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2632" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2632" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2632" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2632" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2633" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2633" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2633" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2633" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2633" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2633" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2633" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2634" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2634" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2634" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2634" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2634" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2634" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2634" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2635" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2635" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2635" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2635" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2635" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2635" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2635" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2636" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2636" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2636" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2636" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2636" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2636" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2636" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2637" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2637" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2637" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2637" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2637" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2637" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2637" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2638" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2638" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2638" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2638" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2638" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2638" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2639" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2639" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2639" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2639" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2639" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2639" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2639" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2640" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2640" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2640" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2640" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2640" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2640" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2641" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2641" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2641" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2641" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2641" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2641" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2642" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2642" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2642" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2642" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2642" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2642" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2642" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2643" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2643" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2643" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2643" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2643" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2643" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2644" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2644" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2644" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2644" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2644" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2644" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2645" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2645" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2645" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2645" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2645" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2645" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2645" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2646" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2646" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2646" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2646" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2646" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2646" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2646" s="97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2647" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2647" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2647" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2647" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2647" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2647" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2648" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2648" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2648" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2648" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2648" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2648" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2648" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2649" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2649" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2649" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2649" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2649" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2649" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G2649" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2650" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2650" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2650" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2650" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2650" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2650" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2651" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2651" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2651" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2651" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2651" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2651" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2652" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2652" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2652" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2652" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2652" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2652" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2652" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2653" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2653" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2653" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2653" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2653" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2653" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2653" s="98" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean up the code and added the rank for zone 5
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8389" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8951" uniqueCount="380">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1969,7 +1969,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H1480"/>
+  <dimension ref="A1:H1584"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1306" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1335" sqref="A1335:XFD1335"/>
@@ -32992,7 +32992,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="1473" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1473" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1473" s="48" t="s">
         <v>27</v>
       </c>
@@ -33009,7 +33009,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1474" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1474" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1474" s="70" t="s">
         <v>27</v>
       </c>
@@ -33029,7 +33029,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1475" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1475" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1475" s="48" t="s">
         <v>27</v>
       </c>
@@ -33046,7 +33046,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1476" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1476" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1476" s="48" t="s">
         <v>27</v>
       </c>
@@ -33063,7 +33063,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="1477" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1477" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1477" s="48" t="s">
         <v>27</v>
       </c>
@@ -33080,7 +33080,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="1478" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1478" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1478" s="70" t="s">
         <v>27</v>
       </c>
@@ -33100,7 +33100,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1479" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1479" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1479" s="70" t="s">
         <v>27</v>
       </c>
@@ -33120,7 +33120,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1480" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1480" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1480" s="70" t="s">
         <v>27</v>
       </c>
@@ -33137,6 +33137,1910 @@
         <v>272</v>
       </c>
       <c r="G1480" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1481" spans="2:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1481" s="91"/>
+      <c r="D1481" s="92"/>
+      <c r="F1481" s="93"/>
+      <c r="G1481" s="94"/>
+      <c r="H1481" s="95"/>
+    </row>
+    <row r="1482" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1482" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1482" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1482" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1482" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1482" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1483" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1483" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1483" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1483" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1483" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1483" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="1484" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1484" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1484" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1484" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1484" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1484" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="1485" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1485" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1485" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1485" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1485" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1485" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1486" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1486" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1486" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1486" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1486" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1486" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1487" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1487" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1487" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1487" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1487" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1487" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1488" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1488" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1488" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1488" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1488" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1488" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1488" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1489" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1489" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1489" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1489" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1489" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1489" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1490" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1490" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1490" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1490" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1490" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1490" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="1491" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1491" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1491" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1491" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1491" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1491" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1492" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1492" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1492" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1492" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1492" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1492" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1493" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1493" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1493" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1493" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1493" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1493" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1494" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1494" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1494" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1494" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1494" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1494" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1494" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1495" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1495" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1495" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1495" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1495" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1495" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1495" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1496" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1496" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1496" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1496" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1496" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1496" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="1497" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1497" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1497" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1497" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1497" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1497" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1497" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1498" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1498" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1498" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1498" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1498" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1498" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1498" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1499" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1499" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1499" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1499" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1499" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1499" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1499" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1500" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1500" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1500" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1500" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1500" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1500" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1501" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1501" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1501" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1501" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1501" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1501" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1502" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1502" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1502" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1502" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1502" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1502" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1502" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1503" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1503" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1503" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1503" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1503" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1503" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1503" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1504" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1504" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1504" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1504" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1504" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1504" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1505" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1505" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1505" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1505" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1505" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1505" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1506" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1506" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1506" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1506" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1506" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1506" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="1507" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1507" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1507" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1507" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1507" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1507" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1508" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1508" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1508" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1508" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1508" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1508" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1509" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1509" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1509" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1509" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1509" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1509" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1509" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1510" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1510" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1510" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1510" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1510" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1510" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1510" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1511" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1511" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1511" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1511" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1511" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1511" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1511" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1512" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1512" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1512" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1512" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1512" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1512" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1512" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1513" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1513" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1513" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1513" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1513" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1513" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1513" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1514" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1514" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1514" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1514" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1514" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1514" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1514" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1515" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1515" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1515" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1515" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1515" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1515" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1515" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1516" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1516" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1516" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1516" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1516" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1516" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1516" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1517" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1517" s="96" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1517" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1517" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1517" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1517" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1517" s="97" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1518" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1518" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1518" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1518" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1518" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1518" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1519" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1519" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1519" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1519" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1519" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1519" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1519" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1520" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1520" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1520" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1520" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1520" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1520" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1520" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1521" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1521" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1521" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1521" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1521" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1521" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="1522" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1522" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1522" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1522" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1522" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1522" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1522" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1523" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1523" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1523" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1523" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1523" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1523" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1523" s="97" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1524" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1524" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1524" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1524" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1524" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1524" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1524" s="97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1525" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1525" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1525" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1525" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1525" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1525" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1526" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1526" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1526" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1526" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1526" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1526" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1527" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1527" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1527" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1527" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1527" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1527" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1527" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1528" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1528" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1528" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1528" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1528" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1528" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1528" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1529" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1529" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1529" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1529" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1529" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1529" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1530" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1530" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1530" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1530" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1530" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1530" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="1531" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1531" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1531" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1531" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1531" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1531" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1531" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1532" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1532" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1532" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1532" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1532" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1532" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1532" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1533" spans="2:8" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1533" s="91"/>
+      <c r="D1533" s="92"/>
+      <c r="F1533" s="93"/>
+      <c r="G1533" s="94"/>
+      <c r="H1533" s="95"/>
+    </row>
+    <row r="1534" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1534" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1534" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1534" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1534" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1534" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1534" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1535" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1535" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1535" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1535" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1535" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1535" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1536" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1536" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1536" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1536" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1536" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1536" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="1537" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1537" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1537" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1537" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1537" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1537" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1538" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1538" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1538" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1538" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1538" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1538" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1539" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1539" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1539" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1539" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1539" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1539" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1540" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1540" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1540" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1540" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1540" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1540" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1540" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1541" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1541" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1541" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1541" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1541" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1541" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1541" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1542" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1542" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1542" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1542" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1542" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1542" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="1543" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1543" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1543" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1543" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1543" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1543" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1543" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1544" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1544" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1544" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1544" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1544" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1544" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1544" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1545" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1545" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1545" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1545" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1545" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1545" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1545" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1546" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1546" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1546" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1546" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1546" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1546" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1547" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1547" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1547" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1547" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1547" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1547" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1548" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1548" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1548" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1548" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1548" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1548" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1548" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1549" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1549" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1549" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1549" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1549" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1549" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1549" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1550" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1550" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1550" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1550" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1550" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1550" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1551" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1551" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1551" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1551" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1551" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1551" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1552" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1552" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1552" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1552" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1552" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1552" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="1553" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1553" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1553" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1553" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1553" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1553" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="1554" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1554" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1554" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1554" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1554" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1554" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1554" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1555" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1555" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1555" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1555" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1555" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1555" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1555" s="97" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1556" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1556" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1556" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1556" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1556" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1556" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1557" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1557" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1557" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1557" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1557" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1557" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1558" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1558" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1558" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1558" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1558" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1558" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1558" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1559" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1559" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1559" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1559" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1559" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1559" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1559" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1560" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1560" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1560" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1560" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1560" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1560" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1560" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1561" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1561" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1561" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1561" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1561" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1561" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1561" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1562" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1562" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1562" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1562" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1562" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1562" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1562" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1563" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1563" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1563" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1563" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1563" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1563" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1563" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1564" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1564" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1564" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1564" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1564" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1564" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1564" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1565" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1565" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1565" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1565" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1565" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1565" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1565" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1566" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1566" s="96" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1566" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1566" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1566" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1566" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1566" s="97" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1567" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1567" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1567" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1567" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1567" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1567" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="1568" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1568" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1568" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1568" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1568" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1568" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1568" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1569" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1569" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1569" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1569" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1569" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1569" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1570" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1570" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1570" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1570" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1570" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1570" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="1571" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1571" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1571" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1571" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1571" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1571" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="1572" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1572" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1572" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1572" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1572" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1572" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1573" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1573" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1573" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1573" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1573" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1573" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1574" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1574" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1574" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1574" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1574" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1574" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1575" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1575" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1575" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1575" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1575" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1575" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1575" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1576" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1576" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1576" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1576" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1576" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1576" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1577" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1577" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1577" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1577" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1577" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1577" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1577" s="97" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1578" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1578" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1578" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1578" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1578" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1578" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="1579" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1579" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1579" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1579" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1579" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1579" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1579" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1580" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1580" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1580" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1580" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1580" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1580" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1580" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1581" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1581" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1581" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1581" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1581" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1581" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1582" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1582" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1582" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1582" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1582" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1582" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="1583" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1583" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1583" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1583" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1583" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1583" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1583" s="98" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1584" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1584" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1584" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1584" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="E1584" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1584" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1584" s="98" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit of buttosn being implemented
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8627" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9195" uniqueCount="382">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1160,6 +1160,15 @@
   </si>
   <si>
     <t> 135</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>328A</t>
+  </si>
+  <si>
+    <t>0016</t>
   </si>
 </sst>
 </file>
@@ -1954,10 +1963,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H1516"/>
+  <dimension ref="A1:H1623"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1348" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1374" sqref="G1374"/>
+    <sheetView tabSelected="1" topLeftCell="A1594" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1609" sqref="H1608:N1609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33701,7 +33710,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="1505" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1505" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1505" s="65" t="s">
         <v>27</v>
       </c>
@@ -33721,7 +33730,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1506" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1506" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1506" s="65" t="s">
         <v>27</v>
       </c>
@@ -33741,7 +33750,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1507" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1507" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1507" s="47" t="s">
         <v>27</v>
       </c>
@@ -33758,7 +33767,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="1508" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1508" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1508" s="47" t="s">
         <v>27</v>
       </c>
@@ -33775,7 +33784,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="1509" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1509" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1509" s="65" t="s">
         <v>27</v>
       </c>
@@ -33795,7 +33804,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1510" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1510" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1510" s="65" t="s">
         <v>27</v>
       </c>
@@ -33815,7 +33824,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1511" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1511" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1511" s="47" t="s">
         <v>27</v>
       </c>
@@ -33832,7 +33841,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="1512" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1512" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1512" s="47" t="s">
         <v>27</v>
       </c>
@@ -33849,7 +33858,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1513" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1513" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1513" s="65" t="s">
         <v>27</v>
       </c>
@@ -33869,7 +33878,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1514" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1514" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1514" s="47" t="s">
         <v>27</v>
       </c>
@@ -33886,7 +33895,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="1515" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1515" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1515" s="65" t="s">
         <v>27</v>
       </c>
@@ -33906,7 +33915,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="1516" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1516" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1516" s="65" t="s">
         <v>27</v>
       </c>
@@ -33924,6 +33933,1936 @@
       </c>
       <c r="G1516" s="89" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="1517" spans="2:8" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1517" s="96"/>
+      <c r="C1517" s="82"/>
+      <c r="D1517" s="83"/>
+      <c r="F1517" s="84"/>
+      <c r="G1517" s="85"/>
+      <c r="H1517" s="86"/>
+    </row>
+    <row r="1518" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1518" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1518" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1518" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1518" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1518" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1519" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1519" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1519" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1519" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1519" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1519" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1520" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1520" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1520" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1520" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1520" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1520" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1520" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1521" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1521" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1521" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1521" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1521" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1521" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="1522" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1522" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1522" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1522" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1522" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1522" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1523" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1523" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1523" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1523" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1523" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1523" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1524" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1524" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1524" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1524" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1524" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1524" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1524" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1525" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1525" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1525" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1525" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1525" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1525" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1525" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1526" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1526" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1526" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1526" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1526" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1526" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1526" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1527" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1527" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1527" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1527" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1527" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1527" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="1528" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1528" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1528" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1528" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1528" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1528" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1529" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1529" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1529" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1529" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1529" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1529" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="1530" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1530" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1530" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1530" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1530" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1530" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="1531" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1531" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1531" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1531" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1531" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1531" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="G1531" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1532" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1532" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1532" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1532" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1532" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1532" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="1533" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1533" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1533" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1533" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1533" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1533" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="1534" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1534" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1534" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1534" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1534" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1534" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1535" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1535" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1535" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1535" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1535" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1535" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="1536" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1536" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1536" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1536" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1536" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1536" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="1537" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1537" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1537" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1537" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1537" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1537" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1537" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1538" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1538" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1538" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1538" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1538" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1538" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1539" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1539" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1539" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1539" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1539" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1539" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1540" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1540" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1540" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1540" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1540" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1540" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1540" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1541" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1541" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1541" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1541" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1541" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1541" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1541" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1542" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1542" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1542" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1542" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1542" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1542" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1542" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1543" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1543" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1543" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1543" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1543" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1543" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1543" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1544" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1544" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1544" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1544" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1544" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1544" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="1545" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1545" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1545" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1545" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1545" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1545" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1546" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1546" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1546" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1546" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1546" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1546" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1546" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1547" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1547" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1547" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1547" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1547" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1547" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="1548" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1548" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1548" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1548" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1548" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1548" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1549" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1549" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1549" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1549" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1549" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1549" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="1550" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1550" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1550" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1550" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1550" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1550" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1551" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1551" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1551" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1551" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1551" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1551" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="1552" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1552" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1552" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1552" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1552" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1552" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1553" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1553" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1553" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1553" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1553" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1553" s="13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="1554" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1554" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1554" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1554" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1554" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1554" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1554" s="88" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="1555" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1555" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1555" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1555" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1555" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1555" s="13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="1556" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1556" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1556" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1556" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1556" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1556" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1556" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1557" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1557" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1557" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1557" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1557" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1557" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1558" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1558" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1558" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1558" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1558" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1558" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1558" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1559" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1559" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1559" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1559" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1559" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1559" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1559" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1560" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1560" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1560" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1560" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1560" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1560" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1560" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1561" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1561" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1561" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1561" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1561" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1561" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1561" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1562" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1562" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1562" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1562" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1562" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1562" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1562" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1563" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1563" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1563" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1563" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1563" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1563" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1563" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1564" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1564" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1564" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1564" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1564" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1564" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1565" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1565" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1565" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1565" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1565" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1565" s="13" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="1566" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1566" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1566" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1566" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1566" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1566" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1566" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1567" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1567" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1567" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1567" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1567" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1567" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="1568" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1568" s="87" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1568" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1568" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1568" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1568" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1568" s="88" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1569" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1569" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1569" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1569" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1569" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1569" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1570" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1570" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1570" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1570" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1570" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1570" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1570" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1571" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1571" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1571" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1571" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1571" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1571" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1571" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1572" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1572" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1572" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1572" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1572" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1572" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1573" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1573" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1573" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1573" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1573" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1573" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1573" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1574" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1574" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1574" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1574" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1574" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1574" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="G1574" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1575" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1575" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1575" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1575" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1575" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1575" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="G1575" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1576" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1576" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1576" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1576" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1576" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1576" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G1576" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1577" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1577" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1577" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1577" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1577" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1577" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1577" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1578" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1578" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1578" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1578" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1578" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1578" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1578" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1579" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1579" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1579" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1579" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1579" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1579" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1579" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1580" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1580" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1580" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1580" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1580" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1580" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="1581" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1581" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1581" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1581" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1581" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1581" s="13" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="1582" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1582" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1582" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1582" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1582" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1582" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1582" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1583" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1583" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1583" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1583" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1583" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1583" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="1584" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1584" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1584" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1584" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1584" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1584" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="1585" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1585" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1585" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1585" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1585" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1585" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1585" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1586" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1586" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1586" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1586" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1586" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1586" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1587" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1587" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1587" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1587" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1587" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1587" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G1587" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1588" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1588" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1588" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1588" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1588" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1588" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="1589" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1589" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1589" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1589" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1589" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1589" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1589" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1590" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1590" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1590" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1590" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1590" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1590" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1590" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1591" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1591" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1591" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1591" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1591" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1591" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1592" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1592" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1592" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1592" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1592" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1592" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1593" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1593" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1593" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1593" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1593" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1593" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1593" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1594" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1594" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1594" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1594" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1594" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1594" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1594" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1595" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1595" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1595" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1595" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1595" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1595" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="1596" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1596" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1596" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1596" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1596" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1596" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1597" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1597" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1597" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1597" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1597" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1597" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1597" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1598" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1598" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1598" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1598" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1598" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1598" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="1599" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1599" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1599" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1599" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1599" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1599" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1599" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1600" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1600" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1600" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1600" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1600" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1600" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="G1600" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1601" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1601" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1601" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1601" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1601" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1601" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="1602" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1602" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1602" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1602" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1602" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1602" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="1603" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1603" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1603" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1603" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1603" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1603" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="1604" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1604" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1604" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1604" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1604" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1604" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="1605" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1605" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1605" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1605" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1605" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1605" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="1606" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1606" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1606" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1606" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1606" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1606" s="13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="1607" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1607" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1607" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1607" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1607" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1607" s="13" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="1608" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1608" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1608" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1608" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1608" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1608" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="G1608" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1609" spans="2:8" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1609" s="96"/>
+      <c r="C1609" s="82"/>
+      <c r="D1609" s="83"/>
+      <c r="F1609" s="84"/>
+      <c r="G1609" s="85"/>
+      <c r="H1609" s="86"/>
+    </row>
+    <row r="1610" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1610" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1610" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1610" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1610" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1610" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1611" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1611" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1611" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1611" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1611" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1611" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1612" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1612" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1612" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1612" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1612" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1612" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="1613" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1613" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1613" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1613" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1613" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1613" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1614" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1614" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1614" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1614" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1614" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1614" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="1615" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1615" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1615" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1615" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1615" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1615" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1616" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1616" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1616" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1616" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1616" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1616" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1616" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1617" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1617" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1617" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1617" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1617" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1617" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="1618" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1618" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1618" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1618" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1618" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1618" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1619" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1619" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1619" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1619" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1619" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1619" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="1620" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1620" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1620" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1620" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1620" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1620" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1621" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1621" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1621" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1621" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1621" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1621" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1621" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1622" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1622" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1622" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1622" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1622" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1622" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="1623" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1623" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1623" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1623" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1623" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1623" s="13" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch back to AM-PM time system
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="270" yWindow="30" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11554" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12442" uniqueCount="395">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1206,11 +1211,14 @@
   <si>
     <t>328A</t>
   </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -1268,7 +1276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1351,8 +1359,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1427,6 +1441,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1434,7 +1463,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1748,6 +1777,21 @@
     <xf numFmtId="49" fontId="6" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1760,6 +1804,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1808,7 +1855,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1841,9 +1888,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1876,6 +1940,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2055,11 +2136,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H2115"/>
+  <dimension ref="A1:H2327"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1561" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1565" sqref="A1565:H1584"/>
+      <pane ySplit="1" topLeftCell="A2117" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H2124" sqref="H2124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35878,7 +35959,7 @@
       </c>
       <c r="H1582" s="103"/>
     </row>
-    <row r="1583" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1583" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1583" s="47" t="s">
         <v>158</v>
       </c>
@@ -35902,7 +35983,7 @@
       </c>
       <c r="H1583" s="103"/>
     </row>
-    <row r="1584" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1584" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1584" s="47" t="s">
         <v>158</v>
       </c>
@@ -35926,7 +36007,7 @@
       </c>
       <c r="H1584" s="103"/>
     </row>
-    <row r="1585" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1585" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1585" s="47" t="s">
         <v>86</v>
       </c>
@@ -35989,7 +36070,7 @@
       </c>
       <c r="H1587" s="103"/>
     </row>
-    <row r="1588" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1588" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1588" s="47" t="s">
         <v>86</v>
       </c>
@@ -36010,7 +36091,7 @@
       </c>
       <c r="H1588" s="103"/>
     </row>
-    <row r="1589" spans="1:8" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1589" spans="1:8" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1589" s="47" t="s">
         <v>86</v>
       </c>
@@ -36034,7 +36115,7 @@
       </c>
       <c r="H1589" s="103"/>
     </row>
-    <row r="1590" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1590" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1590" s="46" t="s">
         <v>86</v>
       </c>
@@ -36057,7 +36138,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="1591" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1591" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1591" s="46" t="s">
         <v>86</v>
       </c>
@@ -36143,7 +36224,7 @@
       </c>
       <c r="H1594" s="103"/>
     </row>
-    <row r="1595" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1595" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1595" s="47" t="s">
         <v>90</v>
       </c>
@@ -36212,7 +36293,7 @@
       </c>
       <c r="H1597" s="103"/>
     </row>
-    <row r="1598" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1598" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1598" s="47" t="s">
         <v>90</v>
       </c>
@@ -45686,7 +45767,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2113" s="47" t="s">
         <v>27</v>
       </c>
@@ -45703,7 +45784,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2114" s="65" t="s">
         <v>27</v>
       </c>
@@ -45723,7 +45804,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2115" s="65" t="s">
         <v>27</v>
       </c>
@@ -45741,6 +45822,3750 @@
       </c>
       <c r="G2115" s="89" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="2116" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2116" s="105"/>
+      <c r="C2116" s="106"/>
+      <c r="D2116" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2116" s="108"/>
+      <c r="G2116" s="109"/>
+      <c r="H2116" s="110"/>
+    </row>
+    <row r="2117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2117" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2117" s="11">
+        <v>42590</v>
+      </c>
+      <c r="D2117" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="E2117" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2117" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="G2117" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2118" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2118" s="11">
+        <v>42590</v>
+      </c>
+      <c r="D2118" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="E2118" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2118" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="G2118" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2119" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2119" s="105"/>
+      <c r="C2119" s="106"/>
+      <c r="D2119" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2119" s="108"/>
+      <c r="G2119" s="109"/>
+      <c r="H2119" s="110"/>
+    </row>
+    <row r="2120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2120" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2120" s="11">
+        <v>42590</v>
+      </c>
+    </row>
+    <row r="2121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2121" s="87"/>
+      <c r="G2121" s="88"/>
+    </row>
+    <row r="2122" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2122" s="105"/>
+      <c r="C2122" s="106"/>
+      <c r="D2122" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2122" s="108"/>
+      <c r="G2122" s="109"/>
+      <c r="H2122" s="110"/>
+    </row>
+    <row r="2123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2123" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2123" s="11">
+        <v>42590</v>
+      </c>
+    </row>
+    <row r="2124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2124" s="87"/>
+      <c r="G2124" s="88"/>
+    </row>
+    <row r="2125" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2125" s="105"/>
+      <c r="C2125" s="106"/>
+      <c r="D2125" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2125" s="108"/>
+      <c r="G2125" s="109"/>
+      <c r="H2125" s="110"/>
+    </row>
+    <row r="2126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2126" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2126" s="11">
+        <v>42590</v>
+      </c>
+    </row>
+    <row r="2127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2127" s="87"/>
+      <c r="G2127" s="88"/>
+    </row>
+    <row r="2128" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2128" s="105"/>
+      <c r="C2128" s="106"/>
+      <c r="D2128" s="107" t="s">
+        <v>394</v>
+      </c>
+      <c r="F2128" s="108"/>
+      <c r="G2128" s="109"/>
+      <c r="H2128" s="110"/>
+    </row>
+    <row r="2129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2129" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2129" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2129" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2129" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2129" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2129" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2130" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2130" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2130" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2130" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2130" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2130" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2131" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2131" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2131" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2131" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2131" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2132" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2132" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2132" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2132" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2132" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2133" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2133" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2133" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2133" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2133" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2134" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2134" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2134" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2134" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2134" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2134" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2135" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2135" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2135" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2135" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2135" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2135" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2136" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2136" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2136" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2136" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2136" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2137" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2137" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2137" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2137" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2137" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2138" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2138" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2138" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2138" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2138" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2139" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2139" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2139" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2139" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2139" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2140" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2140" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2140" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2140" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2140" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2140" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2140" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2141" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2141" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2141" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2141" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2141" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2142" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2142" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2142" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2142" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2142" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2143" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2143" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2143" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2143" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2143" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2143" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2144" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2144" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2144" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2144" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2144" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2144" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2145" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2145" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2145" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2145" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2145" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2145" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2145" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2146" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2146" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2146" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2146" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2146" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2146" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2146" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2147" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2147" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2147" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2147" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2147" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2147" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2147" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2148" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2148" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2148" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2148" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2148" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2148" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2148" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2149" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2149" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2149" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2149" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2149" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2149" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2149" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2150" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2150" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2150" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2150" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2150" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2150" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2150" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2151" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2151" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2151" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2151" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2151" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2151" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2152" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2152" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2152" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2152" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2152" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2152" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2153" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2153" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2153" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2153" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2153" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2153" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2154" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2154" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2154" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2154" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2154" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2154" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2155" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2155" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2155" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2155" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2155" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2155" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2155" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2156" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2156" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2156" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2156" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2156" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2156" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="G2156" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2157" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2157" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2157" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2157" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2157" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2157" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2157" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2158" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2158" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2158" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2158" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2158" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2158" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2158" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2159" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2159" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2159" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2159" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2159" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2159" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G2159" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2160" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2160" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2160" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2160" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2160" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2160" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2161" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2161" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2161" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2161" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2161" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2161" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2161" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2162" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2162" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2162" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2162" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2162" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2162" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2162" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2163" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2163" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2163" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2163" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2163" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2163" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2164" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2164" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2164" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2164" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2164" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2164" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2165" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2165" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2165" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2165" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2165" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2165" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2166" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2166" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2166" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2166" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2166" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2166" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2167" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2167" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2167" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2167" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2167" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2167" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2168" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2168" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2168" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2168" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2168" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2168" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2169" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2169" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2169" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2169" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="E2169" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2169" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2169" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2170" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2170" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2170" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2170" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2170" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2170" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2171" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2171" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2171" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2171" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2171" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2171" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2172" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2172" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2172" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2172" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2172" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2172" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2172" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2173" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2173" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2173" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2173" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2173" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2173" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2173" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2174" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2174" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2174" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2174" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2174" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2174" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2174" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2175" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2175" s="105"/>
+      <c r="C2175" s="106"/>
+      <c r="D2175" s="107" t="s">
+        <v>394</v>
+      </c>
+      <c r="F2175" s="108"/>
+      <c r="G2175" s="109"/>
+      <c r="H2175" s="110"/>
+    </row>
+    <row r="2176" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2176" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2176" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2176" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2176" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2176" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2176" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2177" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2177" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2177" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2177" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2177" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2177" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2177" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2178" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2178" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2178" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2178" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2178" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2178" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2179" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2179" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2179" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2179" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2179" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2180" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2180" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2180" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2180" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2180" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2181" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2181" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2181" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2181" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2181" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2181" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2182" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2182" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2182" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2182" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2182" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2182" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2183" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2183" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2183" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2183" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2183" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2184" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2184" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2184" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2184" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2184" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2184" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2185" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2185" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2185" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2185" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2185" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2185" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2186" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2186" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2186" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2186" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2186" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2186" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2187" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2187" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2187" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2187" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2187" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2187" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2187" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2188" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2188" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2188" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2188" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2188" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2188" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2189" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2189" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2189" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2189" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2189" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2189" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2190" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2190" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2190" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2190" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2190" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2190" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2191" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2191" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2191" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2191" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2191" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2191" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2192" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2192" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2192" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2192" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2192" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2192" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2192" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2193" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2193" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2193" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2193" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2193" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2193" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2194" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2194" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2194" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2194" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2194" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2194" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2195" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2195" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2195" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2195" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2195" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2195" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2196" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2196" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2196" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2196" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2196" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2196" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2196" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2197" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2197" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2197" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2197" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2197" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2197" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2198" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2198" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2198" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2198" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2198" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2198" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2199" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2199" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2199" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2199" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2199" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2199" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2200" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2200" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2200" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2200" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2200" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2200" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2201" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2201" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2201" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2201" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2201" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2201" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2202" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2202" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2202" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2202" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2202" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2202" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2202" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2203" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2203" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2203" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2203" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2203" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2203" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="G2203" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2204" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2204" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2204" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2204" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2204" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2204" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2204" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2205" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2205" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2205" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2205" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2205" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2205" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2205" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2206" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2206" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2206" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2206" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2206" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2206" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G2206" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2207" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2207" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2207" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2207" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2207" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2207" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2208" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2208" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2208" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2208" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2208" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2208" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2208" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2209" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2209" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2209" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2209" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2209" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2209" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2209" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2210" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2210" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2210" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2210" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2210" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2210" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2210" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2211" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2211" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2211" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2211" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2211" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2211" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2212" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2212" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2212" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2212" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2212" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2212" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2213" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2213" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2213" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2213" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2213" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2213" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2214" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2214" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2214" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2214" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2214" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2214" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2215" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2215" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2215" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2215" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2215" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2215" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2216" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2216" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2216" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2216" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="E2216" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2216" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2216" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2217" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2217" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2217" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2217" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2217" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2217" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2218" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2218" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2218" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2218" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2218" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2218" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2219" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2219" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2219" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2219" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2219" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2219" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2219" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2220" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2220" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2220" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2220" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2220" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2220" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2220" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2221" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2221" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2221" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2221" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2221" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2221" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2221" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2222" spans="2:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2222" s="112"/>
+      <c r="C2222" s="113"/>
+      <c r="D2222" s="114"/>
+      <c r="F2222" s="114"/>
+      <c r="G2222" s="115"/>
+      <c r="H2222" s="114"/>
+    </row>
+    <row r="2223" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2223" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2223" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2223" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2223" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2223" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2224" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2224" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2224" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2224" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2224" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2224" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2225" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2225" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2225" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2225" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2225" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2225" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2226" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2226" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2226" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2226" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2226" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2226" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2227" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2227" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2227" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2227" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2227" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2227" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2228" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2228" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2228" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2228" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="E2228" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2228" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2228" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2229" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2229" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2229" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2229" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2229" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2229" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2230" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2230" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2230" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2230" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2230" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2230" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2231" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2231" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2231" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2231" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2231" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2231" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2231" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2232" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2232" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2232" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2232" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2232" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2232" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2232" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2233" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2233" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2233" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2233" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2233" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2233" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2233" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2234" spans="2:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2234" s="112"/>
+      <c r="C2234" s="113"/>
+      <c r="D2234" s="114"/>
+      <c r="F2234" s="114"/>
+      <c r="G2234" s="115"/>
+      <c r="H2234" s="114"/>
+    </row>
+    <row r="2235" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2235" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2235" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2235" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2235" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2235" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2236" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2236" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2236" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2236" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2236" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2236" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2237" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2237" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2237" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2237" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2237" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2237" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2238" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2238" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2238" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2238" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2238" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2238" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2239" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2239" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2239" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2239" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2239" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2239" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2240" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2240" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2240" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2240" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="E2240" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2240" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2240" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2241" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2241" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2241" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2241" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2241" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2241" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2242" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2242" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2242" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2242" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2242" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2242" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2243" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2243" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2243" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2243" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2243" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2243" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2243" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2244" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2244" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2244" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2244" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2244" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2244" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2244" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2245" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2245" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2245" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2245" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2245" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2245" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2245" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2246" spans="2:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2246" s="112"/>
+      <c r="C2246" s="113"/>
+      <c r="D2246" s="114"/>
+      <c r="F2246" s="114"/>
+      <c r="G2246" s="115"/>
+      <c r="H2246" s="114"/>
+    </row>
+    <row r="2247" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2247" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2247" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2247" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2247" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2247" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2247" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2248" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2248" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2248" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2248" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2248" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2248" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2248" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2249" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2249" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2249" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2249" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2249" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2249" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2250" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2250" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2250" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2250" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2250" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2250" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2251" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2251" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2251" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2251" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2251" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2251" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2252" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2252" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2252" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2252" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2252" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2252" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2252" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2253" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2253" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2253" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2253" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2253" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2253" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2253" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2254" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2254" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2254" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2254" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2254" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2254" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2255" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2255" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2255" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2255" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2255" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2255" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2256" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2256" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2256" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2256" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2256" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2256" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2257" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2257" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2257" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2257" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2257" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2257" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2258" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2258" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2258" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2258" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2258" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2258" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2258" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2259" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2259" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2259" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2259" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2259" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2259" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2260" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2260" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2260" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2260" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2260" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2260" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2261" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2261" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2261" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2261" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2261" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2261" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2262" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2262" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2262" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2262" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2262" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2262" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2263" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2263" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2263" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2263" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2263" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2263" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2263" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2264" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2264" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2264" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2264" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2264" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2264" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2264" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2265" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2265" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2265" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2265" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2265" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2265" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2265" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2266" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2266" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2266" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2266" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2266" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2266" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2266" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2267" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2267" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2267" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2267" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2267" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2267" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2267" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2268" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2268" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2268" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2268" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2268" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2268" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2268" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2269" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2269" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2269" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2269" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2269" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2269" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2270" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2270" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2270" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2270" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2270" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2270" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2271" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2271" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2271" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2271" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2271" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2271" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2272" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2272" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2272" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2272" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2272" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2272" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2273" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2273" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2273" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2273" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2273" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2273" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2273" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2274" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2274" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2274" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2274" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2274" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2274" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="G2274" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2275" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2275" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2275" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2275" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2275" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2275" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2275" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2276" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2276" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2276" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2276" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2276" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2276" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2276" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2277" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2277" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2277" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2277" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2277" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2277" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G2277" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2278" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2278" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2278" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2278" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2278" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2278" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2279" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2279" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2279" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2279" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2279" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2279" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2279" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2280" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2280" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2280" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2280" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2280" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2280" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2280" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2281" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2281" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2281" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2281" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2281" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2281" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2281" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2282" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2282" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2282" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2282" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2282" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2282" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2283" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2283" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2283" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2283" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2283" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2283" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2284" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2284" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2284" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2284" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2284" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2284" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2285" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2285" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2285" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2285" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2285" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2285" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2286" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2286" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2286" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2286" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2286" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2286" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2287" spans="2:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2287" s="105"/>
+      <c r="C2287" s="106"/>
+      <c r="D2287" s="107" t="s">
+        <v>394</v>
+      </c>
+      <c r="F2287" s="108"/>
+      <c r="G2287" s="109"/>
+      <c r="H2287" s="110"/>
+    </row>
+    <row r="2288" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2288" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2288" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2288" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2288" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2288" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2288" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2289" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2289" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2289" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2289" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2289" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2289" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2289" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2290" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2290" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2290" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2290" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2290" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2290" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2291" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2291" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2291" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2291" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2291" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2291" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2292" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2292" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2292" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2292" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2292" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2292" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2293" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2293" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2293" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2293" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2293" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2293" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2293" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2294" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2294" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2294" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2294" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2294" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2294" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2294" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2295" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2295" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2295" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2295" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2295" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2295" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2296" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2296" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2296" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2296" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2296" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2296" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2297" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2297" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2297" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2297" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2297" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2297" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2298" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2298" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2298" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2298" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2298" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2298" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2299" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2299" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2299" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2299" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2299" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2299" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2299" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2300" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2300" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2300" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2300" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2300" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2300" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2301" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2301" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2301" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2301" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2301" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2301" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2302" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2302" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2302" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2302" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2302" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2302" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2303" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2303" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2303" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2303" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2303" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2303" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2304" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2304" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2304" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2304" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2304" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2304" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2304" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2305" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2305" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2305" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2305" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2305" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2305" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2305" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2306" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2306" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2306" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2306" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2306" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2306" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2306" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2307" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2307" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2307" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2307" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2307" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2307" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2307" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2308" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2308" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2308" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2308" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2308" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2308" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2308" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2309" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2309" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2309" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2309" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2309" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2309" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2309" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2310" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2310" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2310" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2310" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2310" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2310" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2311" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2311" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2311" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2311" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2311" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2311" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2312" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2312" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2312" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2312" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2312" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2312" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2313" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2313" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2313" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2313" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2313" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2313" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2314" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2314" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2314" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2314" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2314" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2314" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2314" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2315" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2315" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2315" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2315" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2315" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2315" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="G2315" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2316" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2316" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2316" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2316" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2316" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2316" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2316" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2317" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2317" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2317" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2317" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2317" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2317" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="G2317" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2318" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2318" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2318" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2318" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2318" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2318" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G2318" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2319" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2319" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2319" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2319" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2319" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2319" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2320" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2320" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2320" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2320" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2320" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2320" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2320" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2321" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2321" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2321" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2321" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2321" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2321" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G2321" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2322" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2322" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2322" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2322" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2322" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2322" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2322" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2323" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2323" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2323" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2323" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2323" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2323" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2324" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2324" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2324" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2324" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2324" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2324" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2325" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2325" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2325" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2325" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2325" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2325" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2326" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2326" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2326" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2326" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2326" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2326" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2327" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2327" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2327" s="11">
+        <v>42591</v>
+      </c>
+      <c r="D2327" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2327" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2327" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -46163,61 +49988,61 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
     </row>
-    <row r="49" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
     </row>
-    <row r="53" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
     </row>
-    <row r="54" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor bug fixes and UI updates
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12745" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13512" uniqueCount="466">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1392,6 +1392,36 @@
   <si>
     <t>Return podium mic, cable and stand to OSG 1014 L</t>
   </si>
+  <si>
+    <t>2130</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>328A</t>
+  </si>
+  <si>
+    <t>2300</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>JHan</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
 </sst>
 </file>
 
@@ -2358,7 +2388,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H2171"/>
+  <dimension ref="A1:H2307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1972" activePane="bottomLeft" state="frozenSplit"/>
@@ -48578,6 +48608,2719 @@
         <v>242</v>
       </c>
       <c r="G2171" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2172" s="105"/>
+      <c r="C2172" s="106"/>
+      <c r="D2172" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2172" s="108"/>
+      <c r="G2172" s="109"/>
+      <c r="H2172" s="110"/>
+    </row>
+    <row r="2173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2173" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2173" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2173" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2173" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2173" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2173" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2174" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2174" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2174" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2174" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2174" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2175" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2175" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2175" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2175" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2175" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2176" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2176" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2176" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2176" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2176" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2177" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2177" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2177" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2177" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2177" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2177" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="G2177" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2178" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2178" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2178" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2178" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2178" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2178" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2179" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2179" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2179" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2179" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2179" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2180" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2180" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2180" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2180" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2180" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2181" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2181" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2181" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2181" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2181" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2182" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2182" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2182" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2182" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2182" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2183" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2183" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2183" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2183" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2183" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="G2183" s="88" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2184" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2184" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2184" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2184" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2184" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2184" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2185" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2185" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2185" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2185" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2185" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2185" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2186" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2186" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2186" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2186" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2186" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2186" s="13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2187" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2187" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2187" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2187" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2187" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2187" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2188" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2188" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2188" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2188" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2188" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2188" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2189" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2189" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2189" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2189" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2189" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2189" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2190" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2190" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2190" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2190" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2190" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2190" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2190" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2191" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2191" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2191" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2191" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2191" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2191" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2191" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2192" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2192" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2192" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2192" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2192" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2192" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2193" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2193" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2193" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2193" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2193" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2193" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2194" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2194" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2194" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2194" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2194" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2194" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2195" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2195" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2195" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2195" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2195" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2196" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2196" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2196" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2196" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2196" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2196" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2196" s="88" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2197" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2197" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2197" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2197" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2197" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2197" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2198" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2198" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2198" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2198" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2198" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2198" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2198" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2199" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2199" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2199" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2199" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2199" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2199" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2199" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2200" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2200" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2200" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2200" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2200" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2200" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2200" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2201" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2201" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2201" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2201" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2201" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2201" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2202" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2202" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2202" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2202" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2202" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2202" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="G2202" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2203" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2203" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2203" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2203" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2203" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2203" s="13" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2204" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2204" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2204" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2204" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2204" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2204" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2204" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2205" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2205" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2205" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2205" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2205" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2205" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="G2205" s="88" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2206" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2206" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2206" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2206" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2206" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2206" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2206" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2207" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2207" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2207" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2207" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2207" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2207" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2208" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2208" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2208" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2208" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2208" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2208" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2209" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2209" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2209" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2209" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2209" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2210" s="132"/>
+      <c r="C2210" s="133"/>
+      <c r="D2210" s="134"/>
+      <c r="F2210" s="134"/>
+      <c r="G2210" s="135"/>
+      <c r="H2210" s="134"/>
+    </row>
+    <row r="2211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2211" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2211" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2211" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2211" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2211" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2211" s="88" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2212" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2212" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2212" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2212" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2212" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2213" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2213" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2213" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2213" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2213" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2214" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2214" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2214" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2214" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2214" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2214" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2215" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2215" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2215" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2215" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2215" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2215" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2216" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2216" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2216" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2216" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2216" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2216" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2217" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2217" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2217" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2217" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2217" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2217" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2218" s="105"/>
+      <c r="C2218" s="106"/>
+      <c r="D2218" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2218" s="108"/>
+      <c r="G2218" s="109"/>
+      <c r="H2218" s="110"/>
+    </row>
+    <row r="2219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2219" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2219" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2219" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2219" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2219" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2219" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2219" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2220" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2220" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2220" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2220" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2220" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2220" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2220" s="88" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2221" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2221" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2221" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2221" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2221" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2221" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2222" s="132"/>
+      <c r="C2222" s="133"/>
+      <c r="D2222" s="134"/>
+      <c r="F2222" s="134"/>
+      <c r="G2222" s="135"/>
+      <c r="H2222" s="134"/>
+    </row>
+    <row r="2223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2223" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2223" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2223" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2223" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2223" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2223" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2224" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2224" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2224" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2224" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2224" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2224" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2224" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2225" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2225" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2225" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2225" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2225" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2225" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2225" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2226" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2226" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2226" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2226" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2226" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2226" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2226" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2227" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2227" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2227" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2227" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2227" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2227" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2227" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2228" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2228" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2228" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2228" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2228" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2228" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2228" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2229" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2229" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2229" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2229" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2229" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2229" s="13" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2230" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2230" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2230" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2230" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2230" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2230" s="13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2231" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2231" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2231" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2231" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2231" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2231" s="13" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2232" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2232" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2232" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2232" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2232" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2232" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2232" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2233" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2233" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2233" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2233" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2233" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2233" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2233" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2234" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2234" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2234" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2234" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2234" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2234" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2234" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2235" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2235" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2235" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2235" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2235" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2235" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2236" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2236" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2236" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2236" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2236" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2236" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2237" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2237" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2237" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2237" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2237" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2237" s="13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2238" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2238" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2238" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2238" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2238" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2238" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2238" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2239" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2239" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2239" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2239" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2239" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2239" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2239" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2240" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2240" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2240" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2240" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2240" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2240" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2240" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2241" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2241" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2241" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2241" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="E2241" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2241" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="G2241" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2242" s="105"/>
+      <c r="C2242" s="106"/>
+      <c r="D2242" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2242" s="108"/>
+      <c r="G2242" s="109"/>
+      <c r="H2242" s="110"/>
+    </row>
+    <row r="2243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2243" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2243" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2243" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2243" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2243" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2243" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2243" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2244" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2244" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2244" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2244" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2244" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2244" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2244" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2245" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2245" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2245" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2245" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2245" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2245" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2246" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2246" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2246" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2246" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2246" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2246" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2247" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2247" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2247" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2247" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2247" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2247" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2248" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2248" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2248" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2248" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2248" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2248" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="G2248" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2249" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2249" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2249" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2249" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2249" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2249" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2250" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2250" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2250" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2250" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2250" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2250" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2251" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2251" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2251" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2251" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2251" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2251" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2252" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2252" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2252" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2252" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2252" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2252" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2253" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2253" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2253" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2253" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2253" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2253" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2254" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2254" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2254" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2254" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2254" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2254" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2255" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2255" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2255" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2255" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2255" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2255" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="G2255" s="88" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2256" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2256" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2256" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2256" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2256" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2256" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2257" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2257" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2257" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2257" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2257" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2257" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2258" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2258" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2258" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2258" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2258" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2258" s="13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2259" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2259" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2259" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2259" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2259" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2259" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2260" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2260" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2260" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2260" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2260" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2260" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2261" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2261" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2261" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2261" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2261" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2261" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2262" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2262" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2262" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2262" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2262" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2262" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2262" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2263" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2263" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2263" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2263" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2263" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2263" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2263" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2264" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2264" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2264" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2264" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2264" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2264" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2265" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2265" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2265" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2265" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2265" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2265" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="G2265" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2266" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2266" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2266" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2266" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2266" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2266" s="13" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2267" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2267" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2267" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2267" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2267" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2267" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2267" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2268" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2268" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2268" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2268" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2268" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2268" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="G2268" s="88" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2269" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2269" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2269" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2269" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2269" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2269" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2269" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2270" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2270" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2270" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2270" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2270" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2270" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2270" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2271" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2271" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2271" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2271" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2271" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2271" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2271" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2272" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2272" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2272" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2272" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2272" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2272" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2273" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2273" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2273" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2273" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2273" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2273" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2273" s="88" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2274" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2274" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2274" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2274" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2274" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2274" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2274" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2275" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2275" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2275" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2275" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2275" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2275" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G2275" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2276" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2276" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2276" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2276" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2276" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2276" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2276" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2277" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2277" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2277" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2277" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2277" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2277" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2278" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2278" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2278" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2278" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2278" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2278" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2279" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2279" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2279" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2279" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2279" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2279" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2280" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2280" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2280" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2280" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2280" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2280" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2280" s="88" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2281" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2281" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2281" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2281" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2281" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2281" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2282" s="132"/>
+      <c r="C2282" s="133"/>
+      <c r="D2282" s="134"/>
+      <c r="F2282" s="134"/>
+      <c r="G2282" s="135"/>
+      <c r="H2282" s="134"/>
+    </row>
+    <row r="2283" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2283" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2283" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2283" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2283" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2283" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2283" s="13" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2284" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2284" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2284" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2284" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2284" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2284" s="13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2285" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2285" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2285" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2285" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2285" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2285" s="13" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2286" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2286" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2286" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2286" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2286" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2286" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2286" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2287" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2287" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2287" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2287" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2287" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2287" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2287" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2288" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2288" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2288" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2288" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2288" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2288" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2288" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2289" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2289" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2289" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2289" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2289" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2289" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2289" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2290" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2290" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2290" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2290" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2290" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2290" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2290" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2291" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2291" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2291" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2291" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2291" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2291" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2291" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2292" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2292" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2292" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2292" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2292" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2292" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2293" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2293" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2293" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2293" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2293" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2293" s="13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2294" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2294" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2294" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2294" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2294" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2294" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="G2294" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2295" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2295" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2295" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2295" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2295" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2295" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2295" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2296" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2296" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2296" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2296" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2296" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2296" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2296" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2297" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2297" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2297" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2297" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="E2297" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2297" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="G2297" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2298" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2298" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2298" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2298" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2298" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2298" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2299" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2299" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2299" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2299" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2299" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2299" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2299" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2300" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2300" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2300" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2300" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2300" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2300" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2300" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2301" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2301" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2301" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2301" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2301" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2301" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2302" s="105"/>
+      <c r="C2302" s="106"/>
+      <c r="D2302" s="107" t="s">
+        <v>387</v>
+      </c>
+      <c r="F2302" s="108"/>
+      <c r="G2302" s="109"/>
+      <c r="H2302" s="110"/>
+    </row>
+    <row r="2303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2303" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2303" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2303" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2303" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2303" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2303" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2303" s="88" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2304" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2304" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2304" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2304" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2304" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2304" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2305" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2305" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2305" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2305" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2305" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2305" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2306" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2306" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2306" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2306" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2306" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2306" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2306" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2307" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2307" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2307" s="11">
+        <v>42604</v>
+      </c>
+      <c r="D2307" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2307" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2307" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2307" s="89" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated installer and version number
</commit_message>
<xml_diff>
--- a/CLASSOPS/masterlog.xlsx
+++ b/CLASSOPS/masterlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15107" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16454" uniqueCount="507">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1539,6 +1539,12 @@
   <si>
     <t>Lectern mic, stand and cable. To Stedman 114L.</t>
   </si>
+  <si>
+    <t>JHan</t>
+  </si>
+  <si>
+    <t>Door code 11012*</t>
+  </si>
 </sst>
 </file>
 
@@ -2514,7 +2520,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H2571"/>
+  <dimension ref="A1:H2805"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="915" topLeftCell="A2363" activePane="bottomLeft"/>
@@ -56965,6 +56971,4878 @@
       </c>
       <c r="F2571" s="13" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2572" s="105"/>
+      <c r="C2572" s="106"/>
+      <c r="D2572" s="107" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2572" s="108"/>
+      <c r="G2572" s="109"/>
+      <c r="H2572" s="110"/>
+    </row>
+    <row r="2573" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2573" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2573" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2573" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2573" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2573" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2573" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2574" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2574" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2574" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2574" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2574" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2574" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2575" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2575" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2575" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2575" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2575" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2575" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2575" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2576" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2576" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2576" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2576" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2576" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2576" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2576" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2577" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2577" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2577" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2577" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2577" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2577" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2577" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2578" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2578" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2578" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2578" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2578" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2578" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2578" s="88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2579" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2579" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2579" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2579" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2579" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2579" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2579" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2580" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2580" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2580" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2580" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2580" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2580" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2581" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2581" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2581" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2581" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2581" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2581" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2581" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2582" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2582" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2582" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2582" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2582" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2582" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2582" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2583" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2583" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2583" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2583" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2583" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2583" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2583" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2584" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2584" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2584" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2584" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2584" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2584" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2585" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2585" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2585" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2585" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2585" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2585" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2586" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2586" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2586" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2586" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2586" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2586" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2587" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2587" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2587" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2587" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2587" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2587" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2588" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2588" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2588" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2588" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2588" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2588" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2589" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2589" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2589" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2589" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2589" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2589" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2590" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2590" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2590" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2590" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2590" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2590" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2591" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2591" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2591" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2591" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2591" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2591" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2591" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2592" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2592" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2592" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2592" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2592" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2592" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="G2592" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2593" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2593" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2593" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2593" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2593" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2593" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2593" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2593" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2594" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2594" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2594" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2594" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2594" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2594" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2594" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2595" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2595" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2595" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2595" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2595" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2595" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2596" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2596" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2596" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2596" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2596" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2596" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2597" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2597" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2597" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2597" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2597" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2597" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2598" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2598" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2598" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2598" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2598" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2598" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2599" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2599" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2599" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2599" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2599" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2599" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2599" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2600" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2600" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2600" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2600" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2600" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2600" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2601" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2601" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2601" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2601" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2601" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2601" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2602" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2602" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2602" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2602" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2602" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2602" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2603" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2603" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2603" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2603" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2603" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2603" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2603" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2604" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2604" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2604" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2604" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2604" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2604" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2604" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2605" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2605" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2605" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2605" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2605" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2605" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2605" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2606" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2606" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2606" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2606" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2606" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2606" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2606" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2607" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2607" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2607" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2607" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2607" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2607" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2608" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2608" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2608" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2608" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2608" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2608" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2608" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2609" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2609" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2609" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2609" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2609" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2609" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2610" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2610" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2610" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2610" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2610" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2610" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2611" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2611" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2611" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2611" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2611" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2611" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2612" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2612" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2612" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2612" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2612" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2612" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2613" s="132"/>
+      <c r="C2613" s="133"/>
+      <c r="D2613" s="134"/>
+      <c r="F2613" s="134"/>
+      <c r="G2613" s="135"/>
+      <c r="H2613" s="134"/>
+    </row>
+    <row r="2614" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2614" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2614" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2614" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2614" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2614" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2614" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2615" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2615" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2615" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2615" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2615" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2615" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2616" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2616" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2616" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2616" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2616" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2616" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2617" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2617" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2617" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2617" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2617" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2617" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2618" s="105"/>
+      <c r="C2618" s="106"/>
+      <c r="D2618" s="107" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2618" s="108"/>
+      <c r="G2618" s="109"/>
+      <c r="H2618" s="110"/>
+    </row>
+    <row r="2619" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2619" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2619" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2619" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2619" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2619" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2619" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2620" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2620" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2620" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2620" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2620" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2620" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2621" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2621" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2621" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2621" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2621" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2621" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2621" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2622" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2622" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2622" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2622" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2622" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2622" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2622" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2623" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2623" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2623" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2623" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2623" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2623" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2623" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2624" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2624" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2624" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2624" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2624" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2624" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2624" s="88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2625" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2625" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2625" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2625" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2625" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2625" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2625" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2626" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2626" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2626" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2626" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2626" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2626" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2627" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2627" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2627" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2627" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2627" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2627" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2627" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2628" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2628" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2628" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2628" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2628" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2628" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2628" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2629" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2629" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2629" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2629" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2629" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2629" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2629" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2630" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2630" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2630" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2630" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2630" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2630" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2631" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2631" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2631" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2631" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2631" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2631" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2632" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2632" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2632" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2632" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2632" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2632" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2633" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2633" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2633" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2633" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2633" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2633" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2634" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2634" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2634" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2634" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2634" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2634" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2635" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2635" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2635" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2635" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2635" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2635" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2636" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2636" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2636" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2636" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2636" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2636" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2637" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2637" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2637" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2637" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2637" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2637" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2637" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2638" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2638" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2638" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2638" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2638" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2638" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="G2638" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2639" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2639" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2639" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2639" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2639" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2639" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2639" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2640" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2640" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2640" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2640" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2640" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2640" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2640" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2641" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2641" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2641" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2641" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2641" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2641" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2642" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2642" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2642" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2642" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2642" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2642" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2643" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2643" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2643" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2643" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2643" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2643" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2644" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2644" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2644" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2644" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2644" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2644" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2645" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2645" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2645" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2645" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2645" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2645" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2645" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2646" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2646" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2646" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2646" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2646" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2646" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2647" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2647" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2647" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2647" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2647" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2647" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2648" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2648" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2648" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2648" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2648" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2648" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2649" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2649" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2649" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2649" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2649" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2649" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2649" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2650" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2650" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2650" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2650" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2650" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2650" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2650" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2651" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2651" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2651" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2651" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2651" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2651" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2651" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2652" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2652" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2652" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2652" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2652" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2652" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2652" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2653" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2653" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2653" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2653" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2653" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2653" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2654" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2654" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2654" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2654" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2654" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2654" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2654" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2655" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2655" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2655" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2655" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2655" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2655" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2656" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2656" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2656" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2656" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2656" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2656" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2657" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2657" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2657" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2657" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2657" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2657" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2658" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2658" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2658" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2658" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2658" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2658" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2659" s="132"/>
+      <c r="C2659" s="133"/>
+      <c r="D2659" s="134"/>
+      <c r="F2659" s="134"/>
+      <c r="G2659" s="135"/>
+      <c r="H2659" s="134"/>
+    </row>
+    <row r="2660" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2660" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2660" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2660" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2660" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2660" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2660" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2661" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2661" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2661" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2661" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2661" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2661" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2662" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2662" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2662" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2662" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2662" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2662" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2663" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2663" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2663" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2663" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2663" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2663" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2664" s="105"/>
+      <c r="C2664" s="106"/>
+      <c r="D2664" s="107" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2664" s="108"/>
+      <c r="G2664" s="109"/>
+      <c r="H2664" s="110"/>
+    </row>
+    <row r="2665" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2665" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2665" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2665" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2665" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2665" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2665" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2666" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2666" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2666" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2666" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2666" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2666" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2667" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2667" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2667" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2667" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2667" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2667" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2667" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2668" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2668" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2668" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2668" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2668" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2668" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2668" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2669" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2669" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2669" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2669" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2669" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2669" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2669" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2670" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2670" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2670" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2670" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2670" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2670" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2670" s="88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2671" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2671" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2671" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2671" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2671" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2671" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2671" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2672" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2672" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2672" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2672" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2672" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2672" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2673" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2673" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2673" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2673" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2673" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2673" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2673" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2674" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2674" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2674" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2674" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2674" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2674" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2674" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2675" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2675" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2675" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2675" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2675" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2675" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2675" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2676" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2676" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2676" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2676" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2676" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2676" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2677" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2677" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2677" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2677" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2677" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2677" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2678" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2678" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2678" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2678" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2678" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2678" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2679" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2679" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2679" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2679" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2679" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2679" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2680" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2680" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2680" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2680" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2680" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2680" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2681" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2681" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2681" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2681" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2681" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2681" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2682" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2682" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2682" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2682" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2682" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2682" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2683" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2683" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2683" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2683" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2683" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2683" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2683" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2684" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2684" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2684" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2684" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2684" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2684" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="G2684" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2685" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2685" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2685" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2685" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2685" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2685" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2685" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2686" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2686" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2686" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2686" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2686" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2686" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2686" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2687" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2687" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2687" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2687" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2687" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2687" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2688" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2688" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2688" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2688" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2688" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2688" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2689" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2689" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2689" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2689" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2689" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2689" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2690" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2690" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2690" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2690" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2690" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2690" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2691" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2691" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2691" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2691" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2691" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2691" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2691" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2692" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2692" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2692" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2692" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2692" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2692" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2693" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2693" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2693" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2693" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2693" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2693" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2694" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2694" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2694" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2694" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2694" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2694" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2695" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2695" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2695" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2695" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2695" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2695" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2695" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2696" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2696" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2696" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2696" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2696" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2696" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2696" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2697" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2697" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2697" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2697" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2697" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2697" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2697" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2698" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2698" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2698" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2698" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2698" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2698" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2698" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2699" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2699" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2699" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2699" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2699" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2699" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2700" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2700" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2700" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2700" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2700" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2700" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2700" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2701" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2701" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2701" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2701" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2701" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2701" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2702" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2702" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2702" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2702" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2702" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2702" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2703" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2703" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2703" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2703" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2703" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2703" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2704" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2704" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2704" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2704" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2704" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2704" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2705" s="132"/>
+      <c r="C2705" s="133"/>
+      <c r="D2705" s="134"/>
+      <c r="F2705" s="134"/>
+      <c r="G2705" s="135"/>
+      <c r="H2705" s="134"/>
+    </row>
+    <row r="2706" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2706" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2706" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2706" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2706" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2706" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2706" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2707" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2707" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2707" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2707" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2707" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2707" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2708" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2708" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2708" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2708" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2708" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2708" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2709" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2709" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2709" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2709" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2709" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2709" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2710" s="105"/>
+      <c r="C2710" s="106"/>
+      <c r="D2710" s="107" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2710" s="108"/>
+      <c r="G2710" s="109"/>
+      <c r="H2710" s="110"/>
+    </row>
+    <row r="2711" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2711" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2711" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2711" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2711" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2711" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2711" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2711" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2712" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2712" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2712" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2712" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2712" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2712" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2713" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2713" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2713" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2713" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2713" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2713" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2714" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2714" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2714" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2714" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2714" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2714" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2714" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2715" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2715" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2715" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2715" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2715" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2715" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2716" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2716" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2716" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2716" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2716" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2716" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2717" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2717" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2717" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2717" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2717" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2717" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2718" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2718" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2718" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2718" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2718" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2718" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2719" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2719" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2719" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2719" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2719" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2719" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2719" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2720" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2720" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2720" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2720" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2720" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2720" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2720" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2721" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2721" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2721" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2721" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2721" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2721" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2721" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2722" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2722" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2722" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2722" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2722" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2722" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2723" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2723" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2723" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2723" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2723" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2723" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2723" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2724" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2724" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2724" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2724" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2724" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2724" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2724" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2725" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2725" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2725" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2725" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2725" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2725" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2725" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2726" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2726" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2726" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2726" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2726" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2726" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2726" s="88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2727" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2727" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2727" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2727" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2727" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2727" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2727" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2728" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2728" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2728" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2728" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2728" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2728" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2729" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2729" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2729" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2729" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2729" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2729" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2729" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2730" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2730" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2730" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2730" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2730" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2730" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2730" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2731" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2731" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2731" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2731" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2731" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2731" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2732" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2732" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2732" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2732" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2732" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2732" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2733" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2733" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2733" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2733" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2733" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2733" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2734" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2734" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2734" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2734" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2734" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2734" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2735" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2735" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2735" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2735" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2735" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2735" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2735" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2736" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2736" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2736" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2736" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2736" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2736" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2736" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2737" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2737" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2737" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2737" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2737" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2737" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2737" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2738" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2738" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2738" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2738" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2738" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2738" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2739" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2739" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2739" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2739" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2739" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2739" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2740" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2740" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2740" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2740" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2740" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2740" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2741" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2741" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2741" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2741" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2741" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2741" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2742" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2742" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2742" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2742" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2742" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2742" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2743" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2743" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2743" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2743" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2743" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2743" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2744" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2744" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2744" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2744" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2744" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2744" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2745" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2745" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2745" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2745" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2745" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2745" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2745" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2746" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2746" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2746" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2746" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2746" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2746" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="G2746" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2747" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2747" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2747" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2747" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2747" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2747" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2747" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2748" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2748" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2748" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2748" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2748" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2748" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2748" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2749" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2749" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2749" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2749" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2749" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2749" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2750" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2750" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2750" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2750" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2750" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2750" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2751" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2751" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2751" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2751" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2751" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2751" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2752" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2752" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2752" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2752" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2752" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2752" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2753" s="105"/>
+      <c r="C2753" s="106"/>
+      <c r="D2753" s="107" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2753" s="108"/>
+      <c r="G2753" s="109"/>
+      <c r="H2753" s="110"/>
+    </row>
+    <row r="2754" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2754" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2754" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2754" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2754" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2754" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2754" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2755" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2755" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2755" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2755" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2755" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2755" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2756" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2756" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2756" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2756" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2756" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2756" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2756" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2757" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2757" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2757" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2757" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2757" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2757" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2758" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2758" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2758" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2758" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2758" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2758" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2759" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2759" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2759" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2759" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2759" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2759" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2760" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2760" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2760" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2760" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2760" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2760" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2761" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2761" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2761" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2761" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2761" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2761" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2761" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2762" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2762" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2762" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2762" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2762" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2762" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2762" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:8" s="104" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2763" s="105"/>
+      <c r="C2763" s="106"/>
+      <c r="D2763" s="107" t="s">
+        <v>415</v>
+      </c>
+      <c r="F2763" s="108"/>
+      <c r="G2763" s="109"/>
+      <c r="H2763" s="110"/>
+    </row>
+    <row r="2764" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2764" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2764" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2764" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2764" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2764" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2764" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2764" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2765" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2765" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2765" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2765" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2765" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2765" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2766" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2766" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2766" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2766" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2766" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2766" s="13" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2767" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2767" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2767" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2767" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2767" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2767" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2767" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2768" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2768" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2768" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2768" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2768" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2768" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2769" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2769" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2769" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2769" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2769" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2769" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2770" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2770" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2770" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2770" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2770" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2770" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2770" s="36" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2771" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2771" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2771" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2771" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2771" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2771" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2772" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2772" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2772" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2772" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2772" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2772" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2772" s="88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2773" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2773" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2773" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2773" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2773" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2773" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="G2773" s="88" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2774" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2774" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2774" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2774" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2774" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2774" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2774" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2775" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2775" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2775" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2775" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2775" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2775" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2776" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2776" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2776" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2776" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2776" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F2776" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2776" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2777" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2777" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2777" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2777" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2777" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2777" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G2777" s="88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2778" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2778" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2778" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2778" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2778" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2778" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2778" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2779" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2779" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2779" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2779" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2779" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2779" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2779" s="88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2780" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2780" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2780" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2780" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2780" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2780" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2780" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2781" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2781" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2781" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2781" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2781" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2781" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2782" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2782" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2782" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2782" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2782" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2782" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2782" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2783" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2783" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2783" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2783" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2783" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2783" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G2783" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2784" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2784" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2784" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2784" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2784" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2784" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2785" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2785" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2785" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2785" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2785" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2785" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2786" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2786" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2786" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2786" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2786" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2786" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2787" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2787" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2787" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2787" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2787" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2787" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2788" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2788" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2788" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2788" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2788" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2788" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2788" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2789" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2789" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2789" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2789" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2789" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2789" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2789" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2790" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2790" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2790" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2790" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2790" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2790" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2790" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2791" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2791" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2791" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2791" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2791" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2791" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2792" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2792" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2792" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2792" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2792" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2792" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2793" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2793" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2793" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2793" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2793" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2793" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2794" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2794" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2794" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2794" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2794" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2794" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2795" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2795" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2795" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2795" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2795" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2795" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2796" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2796" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2796" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2796" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2796" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2796" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2797" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2797" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2797" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2797" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2797" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2797" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2798" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2798" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2798" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2798" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2798" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2798" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2798" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2799" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2799" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2799" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2799" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2799" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2799" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="G2799" s="89" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2800" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2800" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2800" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2800" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2800" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2800" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2800" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2801" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2801" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2801" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2801" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2801" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2801" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2801" s="88" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2802" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2802" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2802" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2802" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2802" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2802" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2803" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2803" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2803" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2803" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2803" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2803" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2804" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2804" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2804" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2804" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2804" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2804" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2804" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2805" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2805" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2805" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2805" s="11">
+        <v>42615</v>
+      </c>
+      <c r="D2805" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2805" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2805" s="13" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>